<commit_message>
Implemented output of sq_index and its avg pin colors
</commit_message>
<xml_diff>
--- a/quartiles.xlsx
+++ b/quartiles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,32 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>25th Percentile</t>
+          <t>Low_R</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>75th Percentile</t>
+          <t>Low_G</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Low_B</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>High_R</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>High_G</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>High_B</t>
         </is>
       </c>
     </row>
@@ -454,315 +474,483 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>[207. 122.  62.]</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>[220.   173.25 145.  ]</t>
-        </is>
+      <c r="B2" t="n">
+        <v>62</v>
+      </c>
+      <c r="C2" t="n">
+        <v>122</v>
+      </c>
+      <c r="D2" t="n">
+        <v>207</v>
+      </c>
+      <c r="E2" t="n">
+        <v>145</v>
+      </c>
+      <c r="F2" t="n">
+        <v>173</v>
+      </c>
+      <c r="G2" t="n">
+        <v>220</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>[194. 152. 157.]</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>[216.5 177.5 185. ]</t>
-        </is>
+      <c r="B3" t="n">
+        <v>157</v>
+      </c>
+      <c r="C3" t="n">
+        <v>152</v>
+      </c>
+      <c r="D3" t="n">
+        <v>194</v>
+      </c>
+      <c r="E3" t="n">
+        <v>185</v>
+      </c>
+      <c r="F3" t="n">
+        <v>178</v>
+      </c>
+      <c r="G3" t="n">
+        <v>216</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>[170.   170.75 218.75]</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>[180.75 179.75 228.75]</t>
-        </is>
+      <c r="B4" t="n">
+        <v>219</v>
+      </c>
+      <c r="C4" t="n">
+        <v>171</v>
+      </c>
+      <c r="D4" t="n">
+        <v>170</v>
+      </c>
+      <c r="E4" t="n">
+        <v>229</v>
+      </c>
+      <c r="F4" t="n">
+        <v>180</v>
+      </c>
+      <c r="G4" t="n">
+        <v>181</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>[180.   206.   159.25]</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>[185. 213. 167.]</t>
-        </is>
+      <c r="B5" t="n">
+        <v>159</v>
+      </c>
+      <c r="C5" t="n">
+        <v>206</v>
+      </c>
+      <c r="D5" t="n">
+        <v>180</v>
+      </c>
+      <c r="E5" t="n">
+        <v>167</v>
+      </c>
+      <c r="F5" t="n">
+        <v>213</v>
+      </c>
+      <c r="G5" t="n">
+        <v>185</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>[124. 114. 216.]</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>[184. 179. 237.]</t>
-        </is>
+      <c r="B6" t="n">
+        <v>216</v>
+      </c>
+      <c r="C6" t="n">
+        <v>114</v>
+      </c>
+      <c r="D6" t="n">
+        <v>124</v>
+      </c>
+      <c r="E6" t="n">
+        <v>237</v>
+      </c>
+      <c r="F6" t="n">
+        <v>179</v>
+      </c>
+      <c r="G6" t="n">
+        <v>184</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>[128. 135. 221.]</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>[232. 234. 245.]</t>
-        </is>
+      <c r="B7" t="n">
+        <v>221</v>
+      </c>
+      <c r="C7" t="n">
+        <v>135</v>
+      </c>
+      <c r="D7" t="n">
+        <v>128</v>
+      </c>
+      <c r="E7" t="n">
+        <v>245</v>
+      </c>
+      <c r="F7" t="n">
+        <v>234</v>
+      </c>
+      <c r="G7" t="n">
+        <v>232</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>[186. 233. 246.]</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>[207. 240. 252.]</t>
-        </is>
+      <c r="B8" t="n">
+        <v>246</v>
+      </c>
+      <c r="C8" t="n">
+        <v>233</v>
+      </c>
+      <c r="D8" t="n">
+        <v>186</v>
+      </c>
+      <c r="E8" t="n">
+        <v>252</v>
+      </c>
+      <c r="F8" t="n">
+        <v>240</v>
+      </c>
+      <c r="G8" t="n">
+        <v>207</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>[189. 185. 146.]</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>[220.  215.5 178. ]</t>
-        </is>
+      <c r="B9" t="n">
+        <v>146</v>
+      </c>
+      <c r="C9" t="n">
+        <v>185</v>
+      </c>
+      <c r="D9" t="n">
+        <v>189</v>
+      </c>
+      <c r="E9" t="n">
+        <v>178</v>
+      </c>
+      <c r="F9" t="n">
+        <v>216</v>
+      </c>
+      <c r="G9" t="n">
+        <v>220</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>[184. 202. 154.]</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>[197.  214.  173.5]</t>
-        </is>
+      <c r="B10" t="n">
+        <v>154</v>
+      </c>
+      <c r="C10" t="n">
+        <v>202</v>
+      </c>
+      <c r="D10" t="n">
+        <v>184</v>
+      </c>
+      <c r="E10" t="n">
+        <v>174</v>
+      </c>
+      <c r="F10" t="n">
+        <v>214</v>
+      </c>
+      <c r="G10" t="n">
+        <v>197</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>[159. 206. 190.]</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>[179.   220.   208.75]</t>
-        </is>
+      <c r="B11" t="n">
+        <v>190</v>
+      </c>
+      <c r="C11" t="n">
+        <v>206</v>
+      </c>
+      <c r="D11" t="n">
+        <v>159</v>
+      </c>
+      <c r="E11" t="n">
+        <v>209</v>
+      </c>
+      <c r="F11" t="n">
+        <v>220</v>
+      </c>
+      <c r="G11" t="n">
+        <v>179</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>[194. 173. 221.]</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>[206.   187.   229.25]</t>
-        </is>
+      <c r="B12" t="n">
+        <v>221</v>
+      </c>
+      <c r="C12" t="n">
+        <v>173</v>
+      </c>
+      <c r="D12" t="n">
+        <v>194</v>
+      </c>
+      <c r="E12" t="n">
+        <v>229</v>
+      </c>
+      <c r="F12" t="n">
+        <v>187</v>
+      </c>
+      <c r="G12" t="n">
+        <v>206</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>[147. 139. 204.]</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>[182. 176. 230.]</t>
-        </is>
+      <c r="B13" t="n">
+        <v>204</v>
+      </c>
+      <c r="C13" t="n">
+        <v>139</v>
+      </c>
+      <c r="D13" t="n">
+        <v>147</v>
+      </c>
+      <c r="E13" t="n">
+        <v>230</v>
+      </c>
+      <c r="F13" t="n">
+        <v>176</v>
+      </c>
+      <c r="G13" t="n">
+        <v>182</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>[174. 124. 176.]</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>[199. 160. 201.]</t>
-        </is>
+      <c r="B14" t="n">
+        <v>176</v>
+      </c>
+      <c r="C14" t="n">
+        <v>124</v>
+      </c>
+      <c r="D14" t="n">
+        <v>174</v>
+      </c>
+      <c r="E14" t="n">
+        <v>201</v>
+      </c>
+      <c r="F14" t="n">
+        <v>160</v>
+      </c>
+      <c r="G14" t="n">
+        <v>199</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>[204. 198. 159.]</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>[214.  207.  172.5]</t>
-        </is>
+      <c r="B15" t="n">
+        <v>159</v>
+      </c>
+      <c r="C15" t="n">
+        <v>198</v>
+      </c>
+      <c r="D15" t="n">
+        <v>204</v>
+      </c>
+      <c r="E15" t="n">
+        <v>172</v>
+      </c>
+      <c r="F15" t="n">
+        <v>207</v>
+      </c>
+      <c r="G15" t="n">
+        <v>214</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>17</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>[211.  184.  139.5]</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>[241.5 222.  194. ]</t>
-        </is>
+      <c r="B16" t="n">
+        <v>140</v>
+      </c>
+      <c r="C16" t="n">
+        <v>184</v>
+      </c>
+      <c r="D16" t="n">
+        <v>211</v>
+      </c>
+      <c r="E16" t="n">
+        <v>194</v>
+      </c>
+      <c r="F16" t="n">
+        <v>222</v>
+      </c>
+      <c r="G16" t="n">
+        <v>242</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>18</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>[135. 136. 219.]</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>[232. 235. 249.]</t>
-        </is>
+      <c r="B17" t="n">
+        <v>219</v>
+      </c>
+      <c r="C17" t="n">
+        <v>136</v>
+      </c>
+      <c r="D17" t="n">
+        <v>135</v>
+      </c>
+      <c r="E17" t="n">
+        <v>249</v>
+      </c>
+      <c r="F17" t="n">
+        <v>235</v>
+      </c>
+      <c r="G17" t="n">
+        <v>232</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>19</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>[150.   197.25 241.  ]</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>[196. 224. 250.]</t>
-        </is>
+      <c r="B18" t="n">
+        <v>241</v>
+      </c>
+      <c r="C18" t="n">
+        <v>197</v>
+      </c>
+      <c r="D18" t="n">
+        <v>150</v>
+      </c>
+      <c r="E18" t="n">
+        <v>250</v>
+      </c>
+      <c r="F18" t="n">
+        <v>224</v>
+      </c>
+      <c r="G18" t="n">
+        <v>196</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>20</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>[199. 171. 136.]</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>[233. 233. 238.]</t>
-        </is>
+      <c r="B19" t="n">
+        <v>136</v>
+      </c>
+      <c r="C19" t="n">
+        <v>171</v>
+      </c>
+      <c r="D19" t="n">
+        <v>199</v>
+      </c>
+      <c r="E19" t="n">
+        <v>238</v>
+      </c>
+      <c r="F19" t="n">
+        <v>233</v>
+      </c>
+      <c r="G19" t="n">
+        <v>233</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>21</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>[120.  98. 183.]</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>[171.   157.75 210.  ]</t>
-        </is>
+      <c r="B20" t="n">
+        <v>183</v>
+      </c>
+      <c r="C20" t="n">
+        <v>98</v>
+      </c>
+      <c r="D20" t="n">
+        <v>120</v>
+      </c>
+      <c r="E20" t="n">
+        <v>210</v>
+      </c>
+      <c r="F20" t="n">
+        <v>158</v>
+      </c>
+      <c r="G20" t="n">
+        <v>171</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>22</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>[125. 209. 216.]</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>[173. 223. 229.]</t>
-        </is>
+      <c r="B21" t="n">
+        <v>216</v>
+      </c>
+      <c r="C21" t="n">
+        <v>209</v>
+      </c>
+      <c r="D21" t="n">
+        <v>125</v>
+      </c>
+      <c r="E21" t="n">
+        <v>229</v>
+      </c>
+      <c r="F21" t="n">
+        <v>223</v>
+      </c>
+      <c r="G21" t="n">
+        <v>173</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>23</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>[135.   107.25 127.  ]</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>[160.   134.75 154.  ]</t>
-        </is>
+      <c r="B22" t="n">
+        <v>127</v>
+      </c>
+      <c r="C22" t="n">
+        <v>107</v>
+      </c>
+      <c r="D22" t="n">
+        <v>135</v>
+      </c>
+      <c r="E22" t="n">
+        <v>154</v>
+      </c>
+      <c r="F22" t="n">
+        <v>135</v>
+      </c>
+      <c r="G22" t="n">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed multiple sources of truth for p_pin_count
</commit_message>
<xml_diff>
--- a/quartiles.xlsx
+++ b/quartiles.xlsx
@@ -1,37 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Desktop\NanoTechnologies_Lab\Phase A\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C778AB3-1397-4DB2-9279-7F6B68313966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="5760" yWindow="12" windowWidth="17280" windowHeight="12108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Low_R</t>
+  </si>
+  <si>
+    <t>Low_G</t>
+  </si>
+  <si>
+    <t>Low_B</t>
+  </si>
+  <si>
+    <t>High_R</t>
+  </si>
+  <si>
+    <t>High_G</t>
+  </si>
+  <si>
+    <t>High_B</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +78,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,536 +402,518 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Low_R</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Low_G</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Low_B</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>High_R</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>High_G</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>High_B</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>62</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>122</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>207</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>145</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>173</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>220</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>157</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>152</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>194</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>185</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>178</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>216</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>219</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>171</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>170</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>229</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>180</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>181</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>159</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>206</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>180</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>167</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>213</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>185</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>216</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>114</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>124</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>237</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>179</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>184</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>221</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>135</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>128</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>245</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>234</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>232</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>246</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>233</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>186</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>252</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>240</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>207</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>146</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>185</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>189</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>178</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>216</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>220</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>154</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>202</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>184</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>174</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>214</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>197</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>190</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>206</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>159</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>209</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>220</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>179</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>221</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>173</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>194</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>229</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>187</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>206</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>204</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>139</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>147</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>230</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>176</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>182</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>176</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>124</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>174</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>201</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>160</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>199</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>159</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>198</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>204</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>172</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>207</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>214</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="n">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>17</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>140</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>184</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>211</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>194</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>222</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>242</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="n">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>18</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>219</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>136</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>135</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>249</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>235</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17">
         <v>232</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="n">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>19</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>241</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>197</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>150</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>250</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>224</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18">
         <v>196</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="n">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>20</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>136</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>171</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>199</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>238</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>233</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19">
         <v>233</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="n">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>21</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>183</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>98</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>120</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>210</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>158</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20">
         <v>171</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="n">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>22</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>216</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>209</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>125</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>229</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>223</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21">
         <v>173</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="n">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>23</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>127</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>107</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>135</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>154</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22">
         <v>135</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22">
         <v>160</v>
       </c>
     </row>

</xml_diff>